<commit_message>
Fixes to mapping and decimals
</commit_message>
<xml_diff>
--- a/Mappings.xlsx
+++ b/Mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Projects\MyGTAP Tools\MyGTAP-ExtraDat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98FB904-9804-41BF-B9C1-37596608BF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6423B0AD-A3F7-428E-97A7-AF823AC52E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{D8548680-C6B4-48E8-BC74-9AFC405306DF}"/>
+    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{D8548680-C6B4-48E8-BC74-9AFC405306DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="520">
   <si>
     <t>ABW</t>
   </si>
@@ -662,18 +662,12 @@
     <t>Bulgaria</t>
   </si>
   <si>
-    <t>Bahamas, The</t>
-  </si>
-  <si>
     <t>Bosnia and Herzegovina</t>
   </si>
   <si>
     <t>Belize</t>
   </si>
   <si>
-    <t>Bolivia</t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
@@ -716,9 +710,6 @@
     <t>Cyprus</t>
   </si>
   <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
     <t>Germany</t>
   </si>
   <si>
@@ -752,9 +743,6 @@
     <t>Gabon</t>
   </si>
   <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
     <t>Georgia</t>
   </si>
   <si>
@@ -764,9 +752,6 @@
     <t>Guinea</t>
   </si>
   <si>
-    <t>Gambia, The</t>
-  </si>
-  <si>
     <t>Guinea-Bissau</t>
   </si>
   <si>
@@ -824,18 +809,12 @@
     <t>Kenya</t>
   </si>
   <si>
-    <t>Kyrgyz Republic</t>
-  </si>
-  <si>
     <t>Cambodia</t>
   </si>
   <si>
     <t>Kiribati</t>
   </si>
   <si>
-    <t>St. Kitts and Nevis</t>
-  </si>
-  <si>
     <t>Kuwait</t>
   </si>
   <si>
@@ -848,9 +827,6 @@
     <t>Libya</t>
   </si>
   <si>
-    <t>St. Lucia</t>
-  </si>
-  <si>
     <t>Sri Lanka</t>
   </si>
   <si>
@@ -974,9 +950,6 @@
     <t>Suriname</t>
   </si>
   <si>
-    <t>Slovak Republic</t>
-  </si>
-  <si>
     <t>Sweden</t>
   </si>
   <si>
@@ -1019,21 +992,9 @@
     <t>Uruguay</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>St. Vincent and the Grenadines</t>
-  </si>
-  <si>
-    <t>Vietnam</t>
-  </si>
-  <si>
     <t>Vanuatu</t>
   </si>
   <si>
-    <t>West Bank and Gaza</t>
-  </si>
-  <si>
     <t>Samoa</t>
   </si>
   <si>
@@ -1169,9 +1130,6 @@
     <t>ALA</t>
   </si>
   <si>
-    <t>ANT</t>
-  </si>
-  <si>
     <t>ATA</t>
   </si>
   <si>
@@ -1271,9 +1229,6 @@
     <t>Afghanistan</t>
   </si>
   <si>
-    <t>Aland Islands</t>
-  </si>
-  <si>
     <t>American Samoa</t>
   </si>
   <si>
@@ -1310,9 +1265,6 @@
     <t>British Indian Ocean Territory</t>
   </si>
   <si>
-    <t>British Virgin Islands</t>
-  </si>
-  <si>
     <t>Cayman Islands</t>
   </si>
   <si>
@@ -1328,30 +1280,15 @@
     <t>Comoros</t>
   </si>
   <si>
-    <t>Congo, Dem. Rep.</t>
-  </si>
-  <si>
-    <t>Congo, Rep.</t>
-  </si>
-  <si>
     <t>Cook Islands</t>
   </si>
   <si>
-    <t>Cote d'Ivoire</t>
-  </si>
-  <si>
     <t>Croatia</t>
   </si>
   <si>
     <t>Cuba</t>
   </si>
   <si>
-    <t>Curacao</t>
-  </si>
-  <si>
-    <t>Egypt, Arab Rep.</t>
-  </si>
-  <si>
     <t>Equatorial Guinea</t>
   </si>
   <si>
@@ -1403,15 +1340,6 @@
     <t>Heard Island and McDonald Islands</t>
   </si>
   <si>
-    <t>Holy See (Vatican City State)</t>
-  </si>
-  <si>
-    <t>Hong Kong SAR, China</t>
-  </si>
-  <si>
-    <t>Iran, Islamic Rep.</t>
-  </si>
-  <si>
     <t>Isle of Man</t>
   </si>
   <si>
@@ -1421,15 +1349,6 @@
     <t>Kazakhstan</t>
   </si>
   <si>
-    <t>Korea, Dem. People's Rep.</t>
-  </si>
-  <si>
-    <t>Korea, Rep.</t>
-  </si>
-  <si>
-    <t>Lao PDR</t>
-  </si>
-  <si>
     <t>Latvia</t>
   </si>
   <si>
@@ -1442,9 +1361,6 @@
     <t>Lithuania</t>
   </si>
   <si>
-    <t>Macao SAR, China</t>
-  </si>
-  <si>
     <t>Madagascar</t>
   </si>
   <si>
@@ -1460,12 +1376,6 @@
     <t>Mayotte</t>
   </si>
   <si>
-    <t>Micronesia, Fed. Sts.</t>
-  </si>
-  <si>
-    <t>Moldova</t>
-  </si>
-  <si>
     <t>Monaco</t>
   </si>
   <si>
@@ -1478,12 +1388,6 @@
     <t>Nauru</t>
   </si>
   <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Netherlands Antilles</t>
-  </si>
-  <si>
     <t>New Caledonia</t>
   </si>
   <si>
@@ -1508,12 +1412,6 @@
     <t>Poland</t>
   </si>
   <si>
-    <t>Réunion</t>
-  </si>
-  <si>
-    <t>Saint Helena</t>
-  </si>
-  <si>
     <t>Saint Pierre and Miquelon</t>
   </si>
   <si>
@@ -1538,30 +1436,18 @@
     <t>South Sudan</t>
   </si>
   <si>
-    <t>St. Martin (French part)</t>
-  </si>
-  <si>
     <t>Svalbard and Jan Mayen</t>
   </si>
   <si>
-    <t>Taiwan, China</t>
-  </si>
-  <si>
     <t>Tajikistan</t>
   </si>
   <si>
-    <t>Tanzania</t>
-  </si>
-  <si>
     <t>Timor-Leste</t>
   </si>
   <si>
     <t>Tokelau</t>
   </si>
   <si>
-    <t>Turkiye</t>
-  </si>
-  <si>
     <t>Turks and Caicos Islands</t>
   </si>
   <si>
@@ -1571,9 +1457,6 @@
     <t>Uzbekistan</t>
   </si>
   <si>
-    <t>Venezuela, RB</t>
-  </si>
-  <si>
     <t>Virgin Islands (U.S.)</t>
   </si>
   <si>
@@ -1583,26 +1466,155 @@
     <t>Western Sahara</t>
   </si>
   <si>
-    <t>Yemen, Rep.</t>
-  </si>
-  <si>
     <t>economy</t>
   </si>
   <si>
     <t>longnames</t>
+  </si>
+  <si>
+    <t>BES</t>
+  </si>
+  <si>
+    <t>BLM</t>
+  </si>
+  <si>
+    <t>Ã…land Islands</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Bolivia, Plurinational State of</t>
+  </si>
+  <si>
+    <t>Bonaire, Sint Eustatius and Saba</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Congo, Democratic Republic of the</t>
+  </si>
+  <si>
+    <t>CÃ´te d'Ivoire</t>
+  </si>
+  <si>
+    <t>CuraÃ§ao</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Holy See</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Iran, Islamic Republic of</t>
+  </si>
+  <si>
+    <t>Korea, Democratic People's Republic of</t>
+  </si>
+  <si>
+    <t>Korea, Republic of</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Lao People's Democratic Republic</t>
+  </si>
+  <si>
+    <t>Macao</t>
+  </si>
+  <si>
+    <t>Micronesia, Federated States of</t>
+  </si>
+  <si>
+    <t>Moldova, Republic of</t>
+  </si>
+  <si>
+    <t>Netherlands, Kingdom of the</t>
+  </si>
+  <si>
+    <t>Palestine, State of</t>
+  </si>
+  <si>
+    <t>RÃ©union</t>
+  </si>
+  <si>
+    <t>Saint BarthÃ©lemy</t>
+  </si>
+  <si>
+    <t>Saint Helena, Ascension and Tristan da Cunha</t>
+  </si>
+  <si>
+    <t>Saint Kitts and Nevis</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
+  </si>
+  <si>
+    <t>Saint Martin (French part)</t>
+  </si>
+  <si>
+    <t>Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Taiwan, Province of China</t>
+  </si>
+  <si>
+    <t>Tanzania, United Republic of</t>
+  </si>
+  <si>
+    <t>TÃ¼rkiye</t>
+  </si>
+  <si>
+    <t>United Kingdom of Great Britain and Northern Ireland</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Venezuela, Bolivarian Republic of</t>
+  </si>
+  <si>
+    <t>Viet Nam</t>
+  </si>
+  <si>
+    <t>Virgin Islands (British)</t>
+  </si>
+  <si>
+    <t>Yemen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF464649"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1625,8 +1637,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1961,10 +1974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B751476D-B049-4B99-A8B6-FE10F4F9F068}">
-  <dimension ref="A1:C249"/>
+  <dimension ref="A1:X250"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1972,367 +1985,373 @@
     <col min="1" max="1" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>516</v>
+        <v>476</v>
       </c>
       <c r="B1" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="C1" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>363</v>
+      </c>
+      <c r="B3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C3" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>345</v>
+      </c>
+      <c r="B6" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C7" t="s">
+        <v>398</v>
+      </c>
+      <c r="X7" s="1"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>343</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>343</v>
-      </c>
-      <c r="C3" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>343</v>
-      </c>
-      <c r="C4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" t="s">
-        <v>343</v>
-      </c>
-      <c r="C5" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>343</v>
-      </c>
-      <c r="C6" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>343</v>
-      </c>
-      <c r="C7" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" t="s">
-        <v>343</v>
-      </c>
-      <c r="C8" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>362</v>
       </c>
       <c r="B9" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="C9" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>364</v>
       </c>
       <c r="B10" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="C10" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
       <c r="C11" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="C12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="C13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>401</v>
+      </c>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
       <c r="C14" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>402</v>
+      </c>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="C15" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="C16" t="s">
-        <v>293</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="C17" t="s">
-        <v>493</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>375</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="C18" t="s">
-        <v>414</v>
+        <v>481</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="C19" t="s">
-        <v>199</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="C20" t="s">
-        <v>417</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="C21" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C22" t="s">
-        <v>213</v>
+        <v>405</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>408</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="C23" t="s">
-        <v>424</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>362</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C24" t="s">
-        <v>425</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>360</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C25" t="s">
-        <v>435</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>346</v>
       </c>
       <c r="B26" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C26" t="s">
-        <v>229</v>
+        <v>406</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="C27" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>388</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="C28" t="s">
-        <v>450</v>
+        <v>482</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>478</v>
       </c>
       <c r="B29" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="C29" t="s">
-        <v>245</v>
+        <v>483</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
       <c r="C30" t="s">
-        <v>249</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C31" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>394</v>
+        <v>366</v>
       </c>
       <c r="B32" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="C32" t="s">
-        <v>471</v>
+        <v>407</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>393</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="C33" t="s">
-        <v>477</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -2340,769 +2359,769 @@
         <v>377</v>
       </c>
       <c r="B34" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C34" t="s">
-        <v>481</v>
+        <v>408</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C35" t="s">
-        <v>336</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>402</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C36" t="s">
-        <v>491</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C37" t="s">
-        <v>265</v>
+        <v>205</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C38" t="s">
-        <v>270</v>
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>185</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C39" t="s">
-        <v>328</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>174</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C40" t="s">
-        <v>321</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>373</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="C41" t="s">
-        <v>508</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>374</v>
+        <v>30</v>
       </c>
       <c r="B42" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C42" t="s">
-        <v>512</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>349</v>
       </c>
       <c r="B43" t="s">
-        <v>356</v>
+        <v>331</v>
       </c>
       <c r="C43" t="s">
-        <v>460</v>
+        <v>409</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
-        <v>356</v>
+        <v>330</v>
       </c>
       <c r="C44" t="s">
-        <v>262</v>
+        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B45" t="s">
-        <v>356</v>
+        <v>330</v>
       </c>
       <c r="C45" t="s">
-        <v>503</v>
+        <v>307</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="C46" t="s">
-        <v>319</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>184</v>
+        <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="C47" t="s">
-        <v>510</v>
+        <v>410</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>33</v>
+        <v>369</v>
       </c>
       <c r="B48" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="C48" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>367</v>
       </c>
       <c r="B49" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="C49" t="s">
-        <v>456</v>
+        <v>412</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="B50" t="s">
-        <v>355</v>
+        <v>332</v>
       </c>
       <c r="C50" t="s">
-        <v>260</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>399</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="C51" t="s">
-        <v>461</v>
+        <v>413</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>355</v>
+        <v>330</v>
       </c>
       <c r="C52" t="s">
-        <v>462</v>
+        <v>484</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>107</v>
+        <v>36</v>
       </c>
       <c r="B53" t="s">
-        <v>355</v>
+        <v>330</v>
       </c>
       <c r="C53" t="s">
-        <v>468</v>
+        <v>485</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>119</v>
+        <v>368</v>
       </c>
       <c r="B54" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="C54" t="s">
-        <v>280</v>
+        <v>414</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>178</v>
+        <v>41</v>
       </c>
       <c r="B55" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="C55" t="s">
-        <v>502</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B56" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
       <c r="C56" t="s">
-        <v>202</v>
+        <v>486</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B57" t="s">
-        <v>354</v>
+        <v>326</v>
       </c>
       <c r="C57" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>347</v>
       </c>
       <c r="B58" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="C58" t="s">
-        <v>228</v>
+        <v>416</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>52</v>
+        <v>348</v>
       </c>
       <c r="B59" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="C59" t="s">
-        <v>439</v>
+        <v>487</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B60" t="s">
-        <v>354</v>
+        <v>333</v>
       </c>
       <c r="C60" t="s">
-        <v>442</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="B61" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="C61" t="s">
-        <v>261</v>
+        <v>488</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
       <c r="B62" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="C62" t="s">
-        <v>469</v>
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="C63" t="s">
-        <v>282</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="B64" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="C64" t="s">
-        <v>281</v>
+        <v>226</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>395</v>
+        <v>48</v>
       </c>
       <c r="B65" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="C65" t="s">
-        <v>473</v>
+        <v>228</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="B66" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
       <c r="C66" t="s">
-        <v>478</v>
+        <v>230</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>400</v>
+        <v>51</v>
       </c>
       <c r="B67" t="s">
-        <v>354</v>
+        <v>328</v>
       </c>
       <c r="C67" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B68" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="C68" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>404</v>
+        <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C69" t="s">
-        <v>492</v>
+        <v>417</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="B70" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="C70" t="s">
-        <v>314</v>
+        <v>418</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
       <c r="B71" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="C71" t="s">
-        <v>499</v>
+        <v>419</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="B72" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="C72" t="s">
-        <v>504</v>
+        <v>420</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>180</v>
+        <v>55</v>
       </c>
       <c r="B73" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="C73" t="s">
-        <v>324</v>
+        <v>421</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>192</v>
+        <v>371</v>
       </c>
       <c r="B74" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
       <c r="C74" t="s">
-        <v>334</v>
+        <v>422</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>193</v>
+        <v>350</v>
       </c>
       <c r="B75" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="C75" t="s">
-        <v>335</v>
+        <v>423</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B76" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="C76" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B77" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="C77" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B78" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="C78" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>375</v>
       </c>
       <c r="B79" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="C79" t="s">
-        <v>250</v>
+        <v>425</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>109</v>
+        <v>358</v>
       </c>
       <c r="B80" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
       <c r="C80" t="s">
-        <v>475</v>
+        <v>426</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>118</v>
+        <v>365</v>
       </c>
       <c r="B81" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="C81" t="s">
-        <v>279</v>
+        <v>427</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>141</v>
+        <v>60</v>
       </c>
       <c r="B82" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="C82" t="s">
-        <v>489</v>
+        <v>234</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>145</v>
+        <v>65</v>
       </c>
       <c r="B83" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="C83" t="s">
-        <v>300</v>
+        <v>490</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>146</v>
+        <v>62</v>
       </c>
       <c r="B84" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="C84" t="s">
-        <v>301</v>
+        <v>235</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>161</v>
+        <v>44</v>
       </c>
       <c r="B85" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="C85" t="s">
-        <v>312</v>
+        <v>224</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>181</v>
+        <v>63</v>
       </c>
       <c r="B86" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="C86" t="s">
-        <v>325</v>
+        <v>236</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>49</v>
+        <v>373</v>
       </c>
       <c r="B87" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="C87" t="s">
-        <v>232</v>
+        <v>428</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B88" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="C88" t="s">
-        <v>437</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>99</v>
+        <v>351</v>
       </c>
       <c r="B89" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C89" t="s">
-        <v>269</v>
+        <v>430</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="B90" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C90" t="s">
-        <v>273</v>
+        <v>240</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>175</v>
+        <v>374</v>
       </c>
       <c r="B91" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C91" t="s">
-        <v>322</v>
+        <v>429</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>384</v>
+        <v>352</v>
       </c>
       <c r="B92" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="C92" t="s">
-        <v>514</v>
+        <v>431</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>359</v>
+        <v>70</v>
       </c>
       <c r="B93" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="C93" t="s">
-        <v>421</v>
+        <v>241</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>30</v>
+        <v>372</v>
       </c>
       <c r="B94" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="C94" t="s">
-        <v>218</v>
+        <v>432</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>364</v>
+        <v>64</v>
       </c>
       <c r="B95" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="C95" t="s">
-        <v>451</v>
+        <v>237</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="B96" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="C96" t="s">
-        <v>275</v>
+        <v>238</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>157</v>
+        <v>71</v>
       </c>
       <c r="B97" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="C97" t="s">
-        <v>495</v>
+        <v>242</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>183</v>
+        <v>75</v>
       </c>
       <c r="B98" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="C98" t="s">
-        <v>327</v>
+        <v>244</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>3</v>
+        <v>376</v>
       </c>
       <c r="B99" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="C99" t="s">
-        <v>196</v>
+        <v>433</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>47</v>
+        <v>393</v>
       </c>
       <c r="B100" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="C100" t="s">
-        <v>230</v>
+        <v>491</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B101" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C101" t="s">
-        <v>440</v>
+        <v>243</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>363</v>
+        <v>72</v>
       </c>
       <c r="B102" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C102" t="s">
-        <v>444</v>
+        <v>492</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B103" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C103" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -3110,1374 +3129,1374 @@
         <v>82</v>
       </c>
       <c r="B104" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="C104" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B105" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="C105" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="B106" t="s">
         <v>340</v>
       </c>
       <c r="C106" t="s">
-        <v>464</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="B107" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="C107" t="s">
-        <v>467</v>
+        <v>493</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="B108" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="C108" t="s">
-        <v>288</v>
+        <v>249</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="B109" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="C109" t="s">
-        <v>307</v>
+        <v>248</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>163</v>
+        <v>353</v>
       </c>
       <c r="B110" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="C110" t="s">
-        <v>313</v>
+        <v>434</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="B111" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="C111" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>358</v>
+        <v>84</v>
       </c>
       <c r="B112" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="C112" t="s">
-        <v>412</v>
+        <v>252</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="B113" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="C113" t="s">
-        <v>200</v>
+        <v>253</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>380</v>
+        <v>87</v>
       </c>
       <c r="B114" t="s">
         <v>342</v>
       </c>
       <c r="C114" t="s">
-        <v>422</v>
+        <v>255</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="B115" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="C115" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>383</v>
+        <v>86</v>
       </c>
       <c r="B116" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C116" t="s">
-        <v>427</v>
+        <v>254</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>381</v>
+        <v>88</v>
       </c>
       <c r="B117" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C117" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>382</v>
+        <v>89</v>
       </c>
       <c r="B118" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C118" t="s">
-        <v>432</v>
+        <v>256</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="B119" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="C119" t="s">
-        <v>445</v>
+        <v>258</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="B120" t="s">
         <v>342</v>
       </c>
       <c r="C120" t="s">
-        <v>447</v>
+        <v>494</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>365</v>
+        <v>94</v>
       </c>
       <c r="B121" t="s">
         <v>342</v>
       </c>
       <c r="C121" t="s">
-        <v>452</v>
+        <v>495</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>390</v>
+        <v>95</v>
       </c>
       <c r="B122" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C122" t="s">
-        <v>454</v>
+        <v>259</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B123" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C123" t="s">
-        <v>264</v>
+        <v>496</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="B124" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C124" t="s">
-        <v>470</v>
+        <v>497</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="B125" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="C125" t="s">
-        <v>474</v>
+        <v>437</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="B126" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C126" t="s">
-        <v>479</v>
+        <v>260</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>370</v>
+        <v>103</v>
       </c>
       <c r="B127" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C127" t="s">
-        <v>482</v>
+        <v>438</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="B128" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C128" t="s">
-        <v>290</v>
+        <v>261</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>397</v>
+        <v>99</v>
       </c>
       <c r="B129" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="C129" t="s">
-        <v>483</v>
+        <v>262</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>396</v>
+        <v>101</v>
       </c>
       <c r="B130" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C130" t="s">
-        <v>484</v>
+        <v>439</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>369</v>
+        <v>104</v>
       </c>
       <c r="B131" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="C131" t="s">
-        <v>486</v>
+        <v>440</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="B132" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C132" t="s">
-        <v>487</v>
+        <v>264</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="B133" t="s">
         <v>342</v>
       </c>
       <c r="C133" t="s">
-        <v>296</v>
+        <v>498</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>398</v>
+        <v>110</v>
       </c>
       <c r="B134" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C134" t="s">
-        <v>488</v>
+        <v>441</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>189</v>
+        <v>123</v>
       </c>
       <c r="B135" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C135" t="s">
-        <v>332</v>
+        <v>274</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="B136" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C136" t="s">
-        <v>308</v>
+        <v>275</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>405</v>
+        <v>111</v>
       </c>
       <c r="B137" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
       <c r="C137" t="s">
-        <v>506</v>
+        <v>266</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="B138" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C138" t="s">
-        <v>320</v>
+        <v>268</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>177</v>
+        <v>116</v>
       </c>
       <c r="B139" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="C139" t="s">
-        <v>323</v>
+        <v>269</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>406</v>
+        <v>113</v>
       </c>
       <c r="B140" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="C140" t="s">
-        <v>509</v>
+        <v>442</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>188</v>
+        <v>380</v>
       </c>
       <c r="B141" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="C141" t="s">
-        <v>330</v>
+        <v>443</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>409</v>
+        <v>121</v>
       </c>
       <c r="B142" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C142" t="s">
-        <v>513</v>
+        <v>444</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="B143" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="C143" t="s">
-        <v>216</v>
+        <v>273</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>164</v>
+        <v>381</v>
       </c>
       <c r="B144" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="C144" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B145" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="C145" t="s">
-        <v>465</v>
+        <v>267</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>125</v>
+        <v>59</v>
       </c>
       <c r="B146" t="s">
-        <v>352</v>
+        <v>329</v>
       </c>
       <c r="C146" t="s">
-        <v>284</v>
+        <v>499</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>191</v>
+        <v>109</v>
       </c>
       <c r="B147" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="C147" t="s">
-        <v>333</v>
+        <v>500</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>378</v>
+        <v>355</v>
       </c>
       <c r="B148" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="C148" t="s">
-        <v>415</v>
+        <v>446</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>6</v>
+        <v>119</v>
       </c>
       <c r="B149" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C149" t="s">
-        <v>198</v>
+        <v>272</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="B150" t="s">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="C150" t="s">
-        <v>211</v>
+        <v>271</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>24</v>
+        <v>379</v>
       </c>
       <c r="B151" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="C151" t="s">
-        <v>212</v>
+        <v>447</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="B152" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
       <c r="C152" t="s">
-        <v>220</v>
+        <v>265</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>38</v>
+        <v>120</v>
       </c>
       <c r="B153" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C153" t="s">
-        <v>222</v>
+        <v>448</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="B154" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C154" t="s">
-        <v>233</v>
+        <v>270</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>385</v>
+        <v>125</v>
       </c>
       <c r="B155" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C155" t="s">
-        <v>443</v>
+        <v>276</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>389</v>
+        <v>132</v>
       </c>
       <c r="B156" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="C156" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="B157" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="C157" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B158" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="C158" t="s">
-        <v>298</v>
+        <v>501</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>137</v>
+        <v>357</v>
       </c>
       <c r="B159" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="C159" t="s">
-        <v>294</v>
+        <v>450</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="B160" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="C160" t="s">
-        <v>311</v>
+        <v>282</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>182</v>
+        <v>128</v>
       </c>
       <c r="B161" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C161" t="s">
-        <v>326</v>
+        <v>279</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>186</v>
+        <v>126</v>
       </c>
       <c r="B162" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="C162" t="s">
-        <v>511</v>
+        <v>277</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="B163" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="C163" t="s">
-        <v>214</v>
+        <v>278</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>91</v>
+        <v>383</v>
       </c>
       <c r="B164" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="C164" t="s">
-        <v>263</v>
+        <v>451</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>77</v>
+        <v>382</v>
       </c>
       <c r="B165" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="C165" t="s">
-        <v>251</v>
+        <v>452</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="B166" t="s">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="C166" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>124</v>
+        <v>356</v>
       </c>
       <c r="B167" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="C167" t="s">
-        <v>283</v>
+        <v>454</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="B168" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="C168" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B169" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="C169" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>401</v>
+        <v>135</v>
       </c>
       <c r="B170" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
       <c r="C170" t="s">
-        <v>498</v>
+        <v>284</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="B171" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="C171" t="s">
-        <v>318</v>
+        <v>455</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>172</v>
+        <v>344</v>
       </c>
       <c r="B172" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="C172" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>187</v>
+        <v>136</v>
       </c>
       <c r="B173" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="C173" t="s">
-        <v>329</v>
+        <v>285</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>376</v>
+        <v>140</v>
       </c>
       <c r="B174" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="C174" t="s">
-        <v>411</v>
+        <v>288</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>4</v>
+        <v>143</v>
       </c>
       <c r="B175" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="C175" t="s">
-        <v>413</v>
+        <v>290</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="B176" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="C176" t="s">
-        <v>209</v>
+        <v>286</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>74</v>
+        <v>138</v>
       </c>
       <c r="B177" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C177" t="s">
-        <v>434</v>
+        <v>287</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B178" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="C178" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>68</v>
+        <v>141</v>
       </c>
       <c r="B179" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C179" t="s">
-        <v>244</v>
+        <v>457</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>84</v>
+        <v>142</v>
       </c>
       <c r="B180" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="C180" t="s">
-        <v>257</v>
+        <v>289</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="B181" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C181" t="s">
-        <v>277</v>
+        <v>323</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="B182" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C182" t="s">
-        <v>485</v>
+        <v>291</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>142</v>
+        <v>386</v>
       </c>
       <c r="B183" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C183" t="s">
-        <v>297</v>
+        <v>503</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="B184" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C184" t="s">
-        <v>497</v>
+        <v>292</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B185" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="C185" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>53</v>
+        <v>147</v>
       </c>
       <c r="B186" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C186" t="s">
-        <v>234</v>
+        <v>294</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>149</v>
+        <v>479</v>
       </c>
       <c r="B187" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="C187" t="s">
-        <v>304</v>
+        <v>504</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>1</v>
+        <v>388</v>
       </c>
       <c r="B188" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C188" t="s">
-        <v>410</v>
+        <v>505</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B189" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C189" t="s">
-        <v>206</v>
+        <v>506</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="B190" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C190" t="s">
-        <v>215</v>
+        <v>507</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>78</v>
+        <v>354</v>
       </c>
       <c r="B191" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C191" t="s">
-        <v>252</v>
+        <v>508</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>80</v>
+        <v>390</v>
       </c>
       <c r="B192" t="s">
         <v>338</v>
       </c>
       <c r="C192" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>111</v>
+        <v>185</v>
       </c>
       <c r="B193" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C193" t="s">
-        <v>274</v>
+        <v>509</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>131</v>
+        <v>189</v>
       </c>
       <c r="B194" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="C194" t="s">
-        <v>289</v>
+        <v>319</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="B195" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="C195" t="s">
-        <v>292</v>
+        <v>459</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="B196" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C196" t="s">
-        <v>271</v>
+        <v>460</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
       <c r="B197" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="C197" t="s">
-        <v>204</v>
+        <v>295</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
       <c r="B198" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="C198" t="s">
-        <v>205</v>
+        <v>297</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="B199" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="C199" t="s">
-        <v>223</v>
+        <v>461</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>34</v>
+        <v>165</v>
       </c>
       <c r="B200" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C200" t="s">
-        <v>433</v>
+        <v>305</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B201" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="C201" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>65</v>
+        <v>151</v>
       </c>
       <c r="B202" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C202" t="s">
-        <v>242</v>
+        <v>298</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>63</v>
+        <v>359</v>
       </c>
       <c r="B203" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
       <c r="C203" t="s">
-        <v>240</v>
+        <v>462</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="B204" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="C204" t="s">
-        <v>241</v>
+        <v>510</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>66</v>
+        <v>162</v>
       </c>
       <c r="B205" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="C205" t="s">
-        <v>243</v>
+        <v>463</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>98</v>
+        <v>152</v>
       </c>
       <c r="B206" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="C206" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>115</v>
+        <v>156</v>
       </c>
       <c r="B207" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C207" t="s">
-        <v>276</v>
+        <v>302</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>121</v>
+        <v>191</v>
       </c>
       <c r="B208" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="C208" t="s">
-        <v>472</v>
+        <v>320</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>126</v>
+        <v>387</v>
       </c>
       <c r="B209" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="C209" t="s">
-        <v>285</v>
+        <v>464</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="B210" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C210" t="s">
-        <v>286</v>
+        <v>465</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>150</v>
+        <v>53</v>
       </c>
       <c r="B211" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="C211" t="s">
-        <v>305</v>
+        <v>231</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="B212" t="s">
-        <v>353</v>
+        <v>325</v>
       </c>
       <c r="C212" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>403</v>
+        <v>149</v>
       </c>
       <c r="B213" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="C213" t="s">
-        <v>501</v>
+        <v>296</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B214" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="C214" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>7</v>
+        <v>389</v>
       </c>
       <c r="B215" t="s">
-        <v>346</v>
+        <v>327</v>
       </c>
       <c r="C215" t="s">
-        <v>416</v>
+        <v>466</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>11</v>
+        <v>163</v>
       </c>
       <c r="B216" t="s">
-        <v>346</v>
+        <v>327</v>
       </c>
       <c r="C216" t="s">
-        <v>418</v>
+        <v>304</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B217" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="C217" t="s">
-        <v>419</v>
+        <v>217</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="B218" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="C218" t="s">
-        <v>225</v>
+        <v>306</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>62</v>
+        <v>178</v>
       </c>
       <c r="B219" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C219" t="s">
-        <v>239</v>
+        <v>511</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>81</v>
+        <v>170</v>
       </c>
       <c r="B220" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C220" t="s">
-        <v>254</v>
+        <v>467</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>83</v>
+        <v>179</v>
       </c>
       <c r="B221" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C221" t="s">
-        <v>256</v>
+        <v>512</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="B222" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C222" t="s">
-        <v>259</v>
+        <v>309</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>95</v>
+        <v>172</v>
       </c>
       <c r="B223" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C223" t="s">
-        <v>266</v>
+        <v>468</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>97</v>
+        <v>168</v>
       </c>
       <c r="B224" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C224" t="s">
-        <v>267</v>
+        <v>308</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>134</v>
+        <v>391</v>
       </c>
       <c r="B225" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="C225" t="s">
-        <v>291</v>
+        <v>469</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="B226" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="C226" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="B227" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="C227" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B228" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="C228" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
@@ -4485,230 +4504,241 @@
         <v>176</v>
       </c>
       <c r="B229" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="C229" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>5</v>
+        <v>171</v>
       </c>
       <c r="B230" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C230" t="s">
-        <v>197</v>
+        <v>310</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B231" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="C231" t="s">
-        <v>331</v>
+        <v>470</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B232" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="C232" t="s">
-        <v>515</v>
+        <v>314</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>10</v>
+        <v>180</v>
       </c>
       <c r="B233" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C233" t="s">
-        <v>201</v>
+        <v>315</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>13</v>
+        <v>181</v>
       </c>
       <c r="B234" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="C234" t="s">
-        <v>203</v>
+        <v>316</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>361</v>
+        <v>5</v>
       </c>
       <c r="B235" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="C235" t="s">
-        <v>436</v>
+        <v>197</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B236" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="C236" t="s">
-        <v>236</v>
+        <v>514</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>379</v>
+        <v>183</v>
       </c>
       <c r="B237" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C237" t="s">
-        <v>448</v>
+        <v>515</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>44</v>
+        <v>392</v>
       </c>
       <c r="B238" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="C238" t="s">
-        <v>227</v>
+        <v>471</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>386</v>
+        <v>182</v>
       </c>
       <c r="B239" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="C239" t="s">
-        <v>453</v>
+        <v>317</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>407</v>
+        <v>184</v>
       </c>
       <c r="B240" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C240" t="s">
-        <v>455</v>
+        <v>472</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>366</v>
+        <v>188</v>
       </c>
       <c r="B241" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="C241" t="s">
-        <v>458</v>
+        <v>318</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>392</v>
+        <v>186</v>
       </c>
       <c r="B242" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="C242" t="s">
-        <v>459</v>
+        <v>516</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>101</v>
+        <v>187</v>
       </c>
       <c r="B243" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C243" t="s">
-        <v>466</v>
+        <v>517</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>105</v>
+        <v>394</v>
       </c>
       <c r="B244" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="C244" t="s">
-        <v>272</v>
+        <v>518</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="B245" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="C245" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>129</v>
+        <v>395</v>
       </c>
       <c r="B246" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="C246" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B247" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="C247" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>367</v>
+        <v>190</v>
       </c>
       <c r="B248" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="C248" t="s">
-        <v>500</v>
+        <v>519</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>31</v>
+        <v>192</v>
       </c>
       <c r="B249" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C249" t="s">
-        <v>219</v>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>193</v>
+      </c>
+      <c r="B250" t="s">
+        <v>341</v>
+      </c>
+      <c r="C250" t="s">
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>